<commit_message>
Overhaul of build system and upgrade of AVR toolchain: start MEGA support.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -86,9 +86,6 @@
     <t>IOPin, IOPort, compile only; does nothing.</t>
   </si>
   <si>
-    <t>IOPin toggle</t>
-  </si>
-  <si>
     <t>IOPort toggle</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>ATmega2560</t>
+  </si>
+  <si>
+    <t>IOPin LED toggle</t>
   </si>
 </sst>
 </file>
@@ -225,19 +225,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,235 +531,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1426</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6">
+        <v>972</v>
+      </c>
+      <c r="D4" s="6">
+        <v>104</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1250</v>
+      </c>
+      <c r="D5" s="6">
+        <v>104</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1256</v>
+      </c>
+      <c r="D6" s="6">
+        <v>104</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6">
+        <v>416</v>
+      </c>
+      <c r="D7" s="6">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1426</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="9">
-        <v>972</v>
-      </c>
-      <c r="D4" s="9">
-        <v>104</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1250</v>
-      </c>
-      <c r="D5" s="9">
-        <v>104</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1256</v>
-      </c>
-      <c r="D6" s="9">
-        <v>104</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="9">
-        <v>416</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C8" s="6">
+        <v>180</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6">
+        <v>162</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
+        <v>290</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6">
+        <v>232</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="9">
-        <v>180</v>
-      </c>
-      <c r="D8" s="9">
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6">
+        <v>362</v>
+      </c>
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9">
-        <v>162</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="9">
-        <v>232</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="9">
-        <v>362</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>1618</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <v>166</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Overhaul of build system and upgrade of AVR toolchain: continue MEGA support.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -521,7 +521,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,8 +717,12 @@
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="6">
+        <v>360</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">

</xml_diff>

<commit_message>
Overhaul of build system and upgrade of AVR toolchain: add ATtiny X4 support. Add ArduinoISP support for upload.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -521,7 +521,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,8 +693,12 @@
       <c r="D9" s="6">
         <v>0</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="6">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
       <c r="G9" s="6">
         <v>290</v>
       </c>

</xml_diff>

<commit_message>
Major refactoring of Board namespace (UNO only) and all dependencies.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Example</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>IOPin LED toggle</t>
+  </si>
+  <si>
+    <t>UartApp2</t>
+  </si>
+  <si>
+    <t>SW UART</t>
+  </si>
+  <si>
+    <t>UartApp3</t>
+  </si>
+  <si>
+    <t>SW UARX/UATX</t>
+  </si>
+  <si>
+    <t>PinChangeInterrupt1</t>
+  </si>
+  <si>
+    <t>PinChangeInterrupt2</t>
+  </si>
+  <si>
+    <t>PinChangeInterrupt3</t>
   </si>
 </sst>
 </file>
@@ -518,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +551,7 @@
     <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -550,7 +571,7 @@
       </c>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="4" t="s">
@@ -572,7 +593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -580,7 +601,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="5">
-        <v>1426</v>
+        <v>1500</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -589,8 +610,14 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" s="5">
+        <v>1426</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -598,7 +625,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="6">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="D4" s="6">
         <v>104</v>
@@ -607,8 +634,14 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J4" s="6">
+        <v>972</v>
+      </c>
+      <c r="K4" s="6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -616,7 +649,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="6">
-        <v>1250</v>
+        <v>1256</v>
       </c>
       <c r="D5" s="6">
         <v>104</v>
@@ -625,8 +658,14 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J5" s="6">
+        <v>1250</v>
+      </c>
+      <c r="K5" s="6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -634,7 +673,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="6">
-        <v>1256</v>
+        <v>1262</v>
       </c>
       <c r="D6" s="6">
         <v>104</v>
@@ -643,8 +682,14 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J6" s="6">
+        <v>1256</v>
+      </c>
+      <c r="K6" s="6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -652,17 +697,17 @@
         <v>19</v>
       </c>
       <c r="C7" s="6">
-        <v>416</v>
+        <v>380</v>
       </c>
       <c r="D7" s="6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -670,7 +715,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="6">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D8" s="6">
         <v>0</v>
@@ -680,7 +725,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -706,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -728,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -736,7 +781,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="6">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="D11" s="6">
         <v>0</v>
@@ -746,7 +791,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -754,25 +799,115 @@
         <v>23</v>
       </c>
       <c r="C12" s="6">
-        <v>1618</v>
+        <v>1884</v>
       </c>
       <c r="D12" s="6">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="3"/>
+      <c r="J12" s="6">
+        <v>1618</v>
+      </c>
+      <c r="K12" s="6">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1628</v>
+      </c>
+      <c r="D13" s="6">
+        <v>158</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1626</v>
+      </c>
+      <c r="D14" s="6">
+        <v>158</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6">
+        <v>514</v>
+      </c>
+      <c r="D15" s="6">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6">
+        <v>704</v>
+      </c>
+      <c r="D16" s="6">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6">
+        <v>486</v>
+      </c>
+      <c r="D17" s="6">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -783,6 +918,6 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring of make (all specifics are now in one file only). Review all samples to include ATtinyX4.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\electronics\projects\FastArduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\electronics\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Example</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>PinChangeInterrupt3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Use PCI on push button to light LED</t>
+  </si>
+  <si>
+    <t>Use PCI on 3 push buttons to light 4 LEDs</t>
   </si>
 </sst>
 </file>
@@ -241,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -258,6 +267,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,7 +554,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,10 +618,18 @@
       <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="2"/>
+      <c r="E3" s="5">
+        <v>1446</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1684</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
       <c r="J3" s="5">
         <v>1426</v>
       </c>
@@ -630,10 +650,18 @@
       <c r="D4" s="6">
         <v>104</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
+      <c r="E4" s="6">
+        <v>954</v>
+      </c>
+      <c r="F4" s="6">
+        <v>104</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1132</v>
+      </c>
+      <c r="H4" s="2">
+        <v>104</v>
+      </c>
       <c r="J4" s="6">
         <v>972</v>
       </c>
@@ -654,10 +682,18 @@
       <c r="D5" s="6">
         <v>104</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="2"/>
+      <c r="E5" s="6">
+        <v>1232</v>
+      </c>
+      <c r="F5" s="6">
+        <v>104</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1410</v>
+      </c>
+      <c r="H5" s="2">
+        <v>104</v>
+      </c>
       <c r="J5" s="6">
         <v>1250</v>
       </c>
@@ -678,10 +714,18 @@
       <c r="D6" s="6">
         <v>104</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="6">
+        <v>1238</v>
+      </c>
+      <c r="F6" s="6">
+        <v>104</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1416</v>
+      </c>
+      <c r="H6" s="2">
+        <v>104</v>
+      </c>
       <c r="J6" s="6">
         <v>1256</v>
       </c>
@@ -702,10 +746,20 @@
       <c r="D7" s="6">
         <v>7</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="2"/>
+      <c r="E7" s="6">
+        <v>310</v>
+      </c>
+      <c r="F7" s="6">
+        <v>7</v>
+      </c>
+      <c r="G7" s="6">
+        <v>522</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -715,15 +769,29 @@
         <v>26</v>
       </c>
       <c r="C8" s="6">
+        <v>156</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>86</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>284</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
         <v>174</v>
       </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -750,6 +818,8 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -764,14 +834,20 @@
       <c r="D10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="6">
+        <v>162</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
       <c r="G10" s="6">
         <v>360</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -786,10 +862,20 @@
       <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="2"/>
+      <c r="E11" s="6">
+        <v>276</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>474</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -804,10 +890,18 @@
       <c r="D12" s="6">
         <v>169</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="2"/>
+      <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2031</v>
+      </c>
+      <c r="H12" s="2">
+        <v>169</v>
+      </c>
       <c r="J12" s="6">
         <v>1618</v>
       </c>
@@ -828,10 +922,20 @@
       <c r="D13" s="6">
         <v>158</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="2"/>
+      <c r="E13" s="6">
+        <v>1584</v>
+      </c>
+      <c r="F13" s="6">
+        <v>158</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1768</v>
+      </c>
+      <c r="H13" s="2">
+        <v>158</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -846,60 +950,106 @@
       <c r="D14" s="6">
         <v>158</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="2"/>
+      <c r="E14" s="6">
+        <v>1582</v>
+      </c>
+      <c r="F14" s="6">
+        <v>158</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1766</v>
+      </c>
+      <c r="H14" s="2">
+        <v>158</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="C15" s="6">
         <v>514</v>
       </c>
       <c r="D15" s="6">
         <v>8</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="2"/>
+      <c r="E15" s="6">
+        <v>430</v>
+      </c>
+      <c r="F15" s="6">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6">
+        <v>652</v>
+      </c>
+      <c r="H15" s="2">
+        <v>8</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="C16" s="6">
         <v>704</v>
       </c>
       <c r="D16" s="6">
         <v>8</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E16" s="6">
+        <v>618</v>
+      </c>
+      <c r="F16" s="6">
+        <v>8</v>
+      </c>
+      <c r="G16" s="6">
+        <v>820</v>
+      </c>
+      <c r="H16" s="2">
+        <v>8</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="C17" s="6">
         <v>486</v>
       </c>
       <c r="D17" s="6">
         <v>8</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="6">
+        <v>408</v>
+      </c>
+      <c r="F17" s="6">
+        <v>8</v>
+      </c>
+      <c r="G17" s="6">
+        <v>626</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>

</xml_diff>

<commit_message>
Update code size repo after Functor refactoring.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jean-François Poilprêt</author>
+  </authors>
+  <commentList>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>With functors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Example</t>
   </si>
@@ -140,8 +164,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +180,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,6 +290,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,9 +301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,7 +320,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -364,6 +395,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -399,6 +447,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -550,42 +615,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.875" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="H1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
@@ -604,8 +673,14 @@
       <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -613,10 +688,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="5">
-        <v>1500</v>
+        <v>1174</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5">
         <v>1446</v>
@@ -631,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="5">
-        <v>1426</v>
+        <v>1500</v>
       </c>
       <c r="K3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -645,10 +720,10 @@
         <v>16</v>
       </c>
       <c r="C4" s="6">
-        <v>978</v>
+        <v>1014</v>
       </c>
       <c r="D4" s="6">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E4" s="6">
         <v>954</v>
@@ -663,13 +738,13 @@
         <v>104</v>
       </c>
       <c r="J4" s="6">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="K4" s="6">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -677,10 +752,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="6">
-        <v>1256</v>
+        <v>1332</v>
       </c>
       <c r="D5" s="6">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E5" s="6">
         <v>1232</v>
@@ -695,13 +770,13 @@
         <v>104</v>
       </c>
       <c r="J5" s="6">
-        <v>1250</v>
+        <v>1256</v>
       </c>
       <c r="K5" s="6">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -709,10 +784,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="6">
-        <v>1262</v>
+        <v>1338</v>
       </c>
       <c r="D6" s="6">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E6" s="6">
         <v>1238</v>
@@ -727,13 +802,13 @@
         <v>104</v>
       </c>
       <c r="J6" s="6">
-        <v>1256</v>
+        <v>1262</v>
       </c>
       <c r="K6" s="6">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -758,10 +833,14 @@
       <c r="H7" s="2">
         <v>7</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" s="6">
+        <v>380</v>
+      </c>
+      <c r="K7" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -787,13 +866,13 @@
         <v>0</v>
       </c>
       <c r="J8" s="6">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -818,10 +897,14 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="6">
+        <v>162</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -846,10 +929,14 @@
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10" s="6">
+        <v>232</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -874,10 +961,14 @@
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J11" s="6">
+        <v>346</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -890,10 +981,10 @@
       <c r="D12" s="6">
         <v>169</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="6">
@@ -903,13 +994,13 @@
         <v>169</v>
       </c>
       <c r="J12" s="6">
-        <v>1618</v>
+        <v>1884</v>
       </c>
       <c r="K12" s="6">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
@@ -934,10 +1025,14 @@
       <c r="H13" s="2">
         <v>158</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13" s="6">
+        <v>1628</v>
+      </c>
+      <c r="K13" s="6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
@@ -962,10 +1057,14 @@
       <c r="H14" s="2">
         <v>158</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J14" s="6">
+        <v>1626</v>
+      </c>
+      <c r="K14" s="6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -990,10 +1089,14 @@
       <c r="H15" s="2">
         <v>8</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J15" s="6">
+        <v>514</v>
+      </c>
+      <c r="K15" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -1018,10 +1121,14 @@
       <c r="H16" s="2">
         <v>8</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J16" s="6">
+        <v>704</v>
+      </c>
+      <c r="K16" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
@@ -1046,10 +1153,14 @@
       <c r="H17" s="2">
         <v>8</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J17" s="6">
+        <v>486</v>
+      </c>
+      <c r="K17" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1058,9 +1169,12 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="3"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
@@ -1069,5 +1183,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Use "on_xxx" naming convention for all virtual handlers. Code cleanup.
</commit_message>
<xml_diff>
--- a/examples-data.xlsx
+++ b/examples-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\electronics\projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\electronics\projects\FastArduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -619,7 +619,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="6">
-        <v>1884</v>
+        <v>1914</v>
       </c>
       <c r="D12" s="6">
         <v>169</v>

</xml_diff>